<commit_message>
Update RiskList v1.0 (draft).xlsx
</commit_message>
<xml_diff>
--- a/Dokumenty/01 - Inception/RiskList v1.0 (draft).xlsx
+++ b/Dokumenty/01 - Inception/RiskList v1.0 (draft).xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studium\OU - PřF\Magisterské\Ročníkový projekt 1\PraxeO\Dokumenty\01 - Inception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E2579CF-D9A2-4972-8BE3-23F035516510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10A0263-E32C-498A-8B3A-696AF240C7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{0407DDAE-8BE7-4712-86E9-36BBAC94D691}"/>
+    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{0407DDAE-8BE7-4712-86E9-36BBAC94D691}"/>
   </bookViews>
   <sheets>
-    <sheet name="List1" sheetId="1" r:id="rId1"/>
+    <sheet name="RiskList" sheetId="1" r:id="rId1"/>
+    <sheet name="Slovníček pojmů" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="224">
   <si>
     <t>ID</t>
   </si>
@@ -378,13 +379,1807 @@
   </si>
   <si>
     <t>Interní/Externí</t>
+  </si>
+  <si>
+    <t>Bezpečnost &amp; právo</t>
+  </si>
+  <si>
+    <r>
+      <t>GDPR</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – evropská pravidla ochrany osobních údajů.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> když ukládáš jména/studenty, musíš vědět proč, jak dlouho a kdo k nim smí.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DPO (Data Protection Officer)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – pověřená osoba pro dohled nad GDPR.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> radí, jak nastavit procesy a řeší incidenty s osobními daty.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DPIA (Data Protection Impact Assessment)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – posouzení vlivu na ochranu osobních údajů.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> kontrolní seznam „kde hrozí únik/dopad“ a jak riziko snížit.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DPA (Data Processing Agreement)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – smlouva o zpracování osobních údajů s dodavatelem.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pokud hostuješ data u cloudu, DPA říká, co smí a nesmí dělat.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>NDA (Non-Disclosure Agreement)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – dohoda o mlčenlivosti.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> externista nesmí vynášet data/procesy ven.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Šifrování „v klidu“ (encryption-at-rest)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – data jsou šifrovaná na disku.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> když někdo získá kopii databáze, neuvidí obsah.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Šifrování „při přenosu“ (encryption-in-transit)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – data jsou šifrovaná při cestě mezi klientem a serverem (HTTPS/TLS).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sniffer na Wi-Fi neuvidí citlivé údaje.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RBAC (Role-Based Access Control)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – přístupy podle rolí.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> „učitel“ vidí posudky, „student“ jen své věci.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Princip „least-privilege“</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – dávej jen minimální nutná práva.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> uživatel nemusí být admin, aby odeslal posudek.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Audit log(y)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – záznamy „kdo co kdy udělal“.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dohledáš, kdo exportoval data včera večer.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Pen-test (penetration test)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – etický „útok“ na systém, aby se našly slabiny.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> specialisté se cíleně pokoušejí prolomit ochrany.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Maskování dat</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – skrytí části hodnot (např. „Jan N., e-mail: j***@…“).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> export pro externistu neobsahuje celé osobní údaje.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Watermark</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – „vodotisk“ v exportu (např. jméno a čas exportéra).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> když unikne PDF, víš, odkud šlo ven.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Retenční politika</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – pravidla, jak dlouho data/logy držíme a co pak.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> logy mazat po 180 dnech, přílohy po 2 letech.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Anonymizace</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – úprava dat tak, aby už nešla spojit s konkrétní osobou.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> statistiky bez identifikátorů studentů.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Práva subjektů údajů</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – právo na přístup, opravu, výmaz atd.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> musíš umět data člověka najít a smazat/opravit.</t>
+    </r>
+  </si>
+  <si>
+    <t>Identita &amp; přihlášení</t>
+  </si>
+  <si>
+    <r>
+      <t>SSO (Single Sign-On)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – jedno přihlášení pro více systémů.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> přihlásíš se univerzitním účtem a máš hotovo.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>LDAP</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – adresář uživatelů (typicky univerzitní).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> systém si z LDAPu načte, kdo je student/učitel.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MFA (Multi-Factor Authentication)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – dvoufaktor (heslo + kód v mobilu).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i když heslo unikne, útočník se bez kódu nepřihlásí.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SAML / OIDC (OpenID Connect)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – standardy pro napojení SSO.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> „řeč“, kterou si univerzitní přihlášení rozumí s aplikací.</t>
+    </r>
+  </si>
+  <si>
+    <t>Architektura, vývoj &amp; kvalita</t>
+  </si>
+  <si>
+    <r>
+      <t>API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – rozhraní pro komunikaci mezi systémy.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> endpoint „/student/123“ vrátí data studenta.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Validační pravidla</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – technická kontrola správnosti dat.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nepustí duplicitní praxi nebo prázdný posudek.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>De-dup (de-duplication)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – odhalení a sloučení duplicit.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dvě stejné praxe → systém nabídne sloučení.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Indexy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – „rejstřík“ pro rychlé hledání v databázi.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> vyhledání praxí podle firmy je pak výrazně rychlejší.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Stránkování (pagination)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – načítání dat po stránkách.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> místo 10 000 položek najednou zobrazíš 50 na stránku.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Asynchronní zpracování (async)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – úlohy běží „na pozadí“.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> velký export se vygeneruje a pošle odkaz e-mailem.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Test pyramid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – většina testů jsou rychlé jednotkové, méně integračních a pár end-to-end.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> rychle chytáš chyby blízko kódu, jen klíčové scénáře testuješ „celkem“.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>CI (Continuous Integration)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – automatické buildy a testy po každé změně.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> push do repa → běží testy → víš, jestli se něco nerozbilo.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>QA (Quality Assurance)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – zajištění kvality (procesy, testy, kontroly).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> definované standardy, test plány, evidence chyb.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Code review / Peer review</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – kolega zkontroluje změny v kódu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> menší šance, že propustíte bezpečnostní díru.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Playwright / TestCafe</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – nástroje na automatizované testy prohlížeče.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> robot „nakliká“ scénář jako uživatel a zkontroluje výsledek.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Design system</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – opakovaně použitelné UI prvky se sjednoceným stylem.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> všechna tlačítka vypadají a chovají se stejně.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Browser-support policy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – seznam podporovaných prohlížečů a verzí.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> garantuješ funkčnost pro Chrome/Firefox/Edge od verze X.</t>
+    </r>
+  </si>
+  <si>
+    <t>DevOps &amp; provoz</t>
+  </si>
+  <si>
+    <r>
+      <t>CDN (Content Delivery Network)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – síť serverů, které rychle servírují statický obsah.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> přílohy a skripty se načítají z nejbližšího uzlu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Autoscaling</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – automatické přidávání/ubírání serverů podle zátěže.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> na začátku semestru se kapacita sama navýší.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Rate-limiting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – omezení počtu požadavků na uživatele/IP.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> robot nepošle 1000 requestů za vteřinu a neshodí službu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3-2-1 zálohy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – 3 kopie dat, na 2 různých médiích, 1 mimo lokalitu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i když shoří serverovna, máš kopii jinde.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>DR test (Disaster Recovery test)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – zkouška, že se dá systém obnovit podle plánu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> nanečisto obnovíš data a měříš, za jak dlouho jedeš.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RPO / RTO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – cíle obnovy.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RPO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> kolik dat maximálně ztratíš (např. 15 min).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>RTO:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> za jak dlouho musí být systém znovu dostupný (např. 2 hod).</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Multi-AZ (Multi-Availability Zone)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – běh ve více oddělených zónách datacentra.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> výpadek jedné zóny službu nezastaví.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Záložní region</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – další geografická oblast pro běh zálohy systému.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> když spadne celý region, přepneš do jiného.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Runbook</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – krok-za-krokem „návod pro incident“.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> co dělat při výpadku, koho volat, jak obnovit.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>S3-like úložiště</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – objektové úložiště pro soubory/přílohy.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> levné, škálovatelné, vhodné na velké množství příloh.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Kvóty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – limity velikosti/počtu souborů na uživatele/projekt.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> student nemůže nahrát 50 GB videí.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Antivir</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – kontrola souborů proti malware.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> zabrání nahrání infikované přílohy.</t>
+    </r>
+  </si>
+  <si>
+    <t>Projektové řízení &amp; procesy</t>
+  </si>
+  <si>
+    <r>
+      <t>BPMN (Business Process Model and Notation)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – standardní „vývojkový“ výkres procesu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jasně vidíš kroky, role a stavy workflow.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SLA (Service Level Agreement)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – dohodnuté úrovně služby.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> „odpovíme do 2 pracovních dnů“, „dostupnost 99,5 %“.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>MoSCoW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – způsob priorizace: Must/Should/Could/Won’t.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> co je nutné, co by mělo být a co klidně počká.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Change control</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – řízení změn rozsahu/funkcí.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> větší změna jde přes schválení, odhad dopadu a nový plán.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Roadmap (produktová mapa)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – plán „co a kdy“ budeme dodávat.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> kvartální pohled na milníky a hlavní funkce.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sprint capping</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – hlídání stropu práce na sprint.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> do sprintu se vejde jen tolik práce, kolik tým reálně zvládne.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>On-call</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – služba „na telefonu“ pro incidenty mimo běžný čas.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> C je primárně on-call, B je zástup.</t>
+    </r>
+  </si>
+  <si>
+    <t>Data &amp; exporty</t>
+  </si>
+  <si>
+    <r>
+      <t>Role-based export</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – kdo co může exportovat záleží na roli.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> student nevyexportuje cizí posudky.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Šifrované ZIPy</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – export do ZIP archivu chráněného heslem/klíčem.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> i kdyby ZIP unikl, bez hesla je k ničemu.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Data lineage</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – „rodokmen“ dat: odkud pochází, jak se měnila.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Prakticky:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dokážeš vysvětlit, proč má závěrečný report určité číslo.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -403,6 +2198,33 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -474,7 +2296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -488,6 +2310,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -825,7 +2659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91461C9F-39B2-4D93-9DDB-2C896CD99BC7}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1720,15 +3554,778 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8FEA1A-63FC-4DA3-A792-4375BAD7D9BD}">
+  <dimension ref="A1:A177"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1" ht="31">
+      <c r="A1" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="7"/>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="8" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="7"/>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="7"/>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="8" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="7"/>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" s="8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" s="7"/>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="7"/>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" s="7"/>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" s="8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" s="7"/>
+    </row>
+    <row r="24" spans="1:1">
+      <c r="A24" s="8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1">
+      <c r="A26" s="7"/>
+    </row>
+    <row r="27" spans="1:1">
+      <c r="A27" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1">
+      <c r="A28" s="9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1">
+      <c r="A29" s="7"/>
+    </row>
+    <row r="30" spans="1:1">
+      <c r="A30" s="8" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1">
+      <c r="A32" s="7"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1">
+      <c r="A34" s="9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1">
+      <c r="A35" s="7"/>
+    </row>
+    <row r="36" spans="1:1">
+      <c r="A36" s="8" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1">
+      <c r="A37" s="9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1">
+      <c r="A38" s="7"/>
+    </row>
+    <row r="39" spans="1:1">
+      <c r="A39" s="8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1">
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" spans="1:1">
+      <c r="A42" s="8" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1">
+      <c r="A43" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1">
+      <c r="A44" s="7"/>
+    </row>
+    <row r="45" spans="1:1">
+      <c r="A45" s="8" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1">
+      <c r="A46" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1">
+      <c r="A47" s="7"/>
+    </row>
+    <row r="48" spans="1:1">
+      <c r="A48" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1">
+      <c r="A49" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" ht="31">
+      <c r="A51" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1">
+      <c r="A52" s="7"/>
+    </row>
+    <row r="53" spans="1:1">
+      <c r="A53" s="8" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1">
+      <c r="A54" s="9" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1">
+      <c r="A55" s="7"/>
+    </row>
+    <row r="56" spans="1:1">
+      <c r="A56" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1">
+      <c r="A57" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1">
+      <c r="A58" s="7"/>
+    </row>
+    <row r="59" spans="1:1">
+      <c r="A59" s="8" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1">
+      <c r="A60" s="9" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1">
+      <c r="A61" s="7"/>
+    </row>
+    <row r="62" spans="1:1">
+      <c r="A62" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1">
+      <c r="A63" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" ht="31">
+      <c r="A65" s="6" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1">
+      <c r="A66" s="7"/>
+    </row>
+    <row r="67" spans="1:1">
+      <c r="A67" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1">
+      <c r="A68" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1">
+      <c r="A69" s="7"/>
+    </row>
+    <row r="70" spans="1:1">
+      <c r="A70" s="8" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1">
+      <c r="A71" s="9" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1">
+      <c r="A72" s="7"/>
+    </row>
+    <row r="73" spans="1:1">
+      <c r="A73" s="8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1">
+      <c r="A74" s="9" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1">
+      <c r="A75" s="7"/>
+    </row>
+    <row r="76" spans="1:1">
+      <c r="A76" s="8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1">
+      <c r="A77" s="9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1">
+      <c r="A78" s="7"/>
+    </row>
+    <row r="79" spans="1:1">
+      <c r="A79" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1">
+      <c r="A80" s="9" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1">
+      <c r="A81" s="7"/>
+    </row>
+    <row r="82" spans="1:1">
+      <c r="A82" s="8" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1">
+      <c r="A83" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1">
+      <c r="A84" s="7"/>
+    </row>
+    <row r="85" spans="1:1">
+      <c r="A85" s="8" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1">
+      <c r="A86" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1">
+      <c r="A87" s="7"/>
+    </row>
+    <row r="88" spans="1:1">
+      <c r="A88" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1">
+      <c r="A89" s="9" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1">
+      <c r="A90" s="7"/>
+    </row>
+    <row r="91" spans="1:1">
+      <c r="A91" s="8" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1">
+      <c r="A92" s="9" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1">
+      <c r="A93" s="7"/>
+    </row>
+    <row r="94" spans="1:1">
+      <c r="A94" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1">
+      <c r="A95" s="9" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1">
+      <c r="A96" s="7"/>
+    </row>
+    <row r="97" spans="1:1">
+      <c r="A97" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1">
+      <c r="A98" s="9" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1">
+      <c r="A99" s="7"/>
+    </row>
+    <row r="100" spans="1:1">
+      <c r="A100" s="8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1">
+      <c r="A101" s="9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1">
+      <c r="A102" s="7"/>
+    </row>
+    <row r="103" spans="1:1">
+      <c r="A103" s="8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1">
+      <c r="A104" s="9" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" ht="31">
+      <c r="A106" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1">
+      <c r="A107" s="7"/>
+    </row>
+    <row r="108" spans="1:1">
+      <c r="A108" s="8" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1">
+      <c r="A109" s="9" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1">
+      <c r="A110" s="7"/>
+    </row>
+    <row r="111" spans="1:1">
+      <c r="A111" s="8" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1">
+      <c r="A112" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="7"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="8" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="9" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="7"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="8" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="9" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="7"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="9" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="7"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="7"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="8" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="9" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="7"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="8" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="7"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="8" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="7"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="8" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="7"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="8" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="7"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" ht="31">
+      <c r="A145" s="6" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="7"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="8" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="7"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="8" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="9" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="7"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="8" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="7"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="8" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="7"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="8" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="7"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="8" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="7"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="168" spans="1:1" ht="31">
+      <c r="A168" s="6" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="7"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="8" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="7"/>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="8" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="7"/>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0c73cd0d-0c25-40ab-80ea-3e9f8fc44d59">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0cab27e2-5f89-44a4-bd92-116f947691cb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1921,21 +4518,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="0c73cd0d-0c25-40ab-80ea-3e9f8fc44d59">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0cab27e2-5f89-44a4-bd92-116f947691cb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A19917E-2530-434B-BEC9-4DA316C9818C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A8A533C-3762-4BB1-B582-2C6C6B2B02E5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0c73cd0d-0c25-40ab-80ea-3e9f8fc44d59"/>
-    <ds:schemaRef ds:uri="0cab27e2-5f89-44a4-bd92-116f947691cb"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1960,9 +4556,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A8A533C-3762-4BB1-B582-2C6C6B2B02E5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A19917E-2530-434B-BEC9-4DA316C9818C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0c73cd0d-0c25-40ab-80ea-3e9f8fc44d59"/>
+    <ds:schemaRef ds:uri="0cab27e2-5f89-44a4-bd92-116f947691cb"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update RiskList v1.0 (draft).xlsx add new sheet
</commit_message>
<xml_diff>
--- a/Dokumenty/01 - Inception/RiskList v1.0 (draft).xlsx
+++ b/Dokumenty/01 - Inception/RiskList v1.0 (draft).xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Studium\OU - PřF\Magisterské\Ročníkový projekt 1\PraxeO\Dokumenty\01 - Inception\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jessi\School\RPR\PraxeO\Dokumenty\01 - Inception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E10A0263-E32C-498A-8B3A-696AF240C7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A44634F-2358-4D49-A406-A62CED9E38B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" activeTab="1" xr2:uid="{0407DDAE-8BE7-4712-86E9-36BBAC94D691}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{0407DDAE-8BE7-4712-86E9-36BBAC94D691}"/>
   </bookViews>
   <sheets>
     <sheet name="RiskList" sheetId="1" r:id="rId1"/>
-    <sheet name="Slovníček pojmů" sheetId="2" r:id="rId2"/>
+    <sheet name="RiskList v2" sheetId="3" r:id="rId2"/>
+    <sheet name="Slovníček pojmů" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="258">
   <si>
     <t>ID</t>
   </si>
@@ -2173,13 +2174,115 @@
       </rPr>
       <t xml:space="preserve"> dokážeš vysvětlit, proč má závěrečný report určité číslo.</t>
     </r>
+  </si>
+  <si>
+    <t>Nezkušenost členů týmu</t>
+  </si>
+  <si>
+    <t>Tým nemá předchozí zkušenosti s vývojem webových aplikací ani s nástroji používanými v projektu.</t>
+  </si>
+  <si>
+    <t>Neznalost frameworků (React, Spring Boot, PostgreSQL)</t>
+  </si>
+  <si>
+    <t>Riziko nepochopení základních principů a ztráty času při řešení technických problémů.</t>
+  </si>
+  <si>
+    <t>Nekompatibilita mezi frontendem a backendem</t>
+  </si>
+  <si>
+    <t>API a UI nemusí být správně sladěné, může docházet k chybám při komunikaci.</t>
+  </si>
+  <si>
+    <t>Potíže s používáním verzovacího systému Git/GitHub</t>
+  </si>
+  <si>
+    <t>Možnost chybného sloučení větví nebo ztráty kódu kvůli nezkušenosti s Gitem.</t>
+  </si>
+  <si>
+    <t>Nepochopení požadavků a chybná analýza</t>
+  </si>
+  <si>
+    <t>Kvůli absenci zkušeností s analýzou může dojít k nejasnému pochopení zadání a špatnému návrhu 6funkcionalit, což povede k přepracování části systému.</t>
+  </si>
+  <si>
+    <t>Problémy s nastavením prostředí a nástrojů</t>
+  </si>
+  <si>
+    <t>Instalace a konfigurace IntelliJ IDEA, PostgreSQL nebo Node.js může být časově náročná.</t>
+  </si>
+  <si>
+    <t>Nedostatečné testování a ladění aplikace</t>
+  </si>
+  <si>
+    <t>Tým nemá zkušenosti s psaním testů ani s debugováním chyb.</t>
+  </si>
+  <si>
+    <t>Problémy s databází a ORM</t>
+  </si>
+  <si>
+    <t>Chyby při návrhu entit nebo relací v PostgreSQL mohou způsobit nefunkčnost aplikace.</t>
+  </si>
+  <si>
+    <t>Zpoždění projektu kvůli nedostatku zkušeností</t>
+  </si>
+  <si>
+    <t>Neznalost nástrojů a metodik zpomalí vývoj, ohrožení termínů.</t>
+  </si>
+  <si>
+    <t>Nízká kvalita kódu a dokumentace</t>
+  </si>
+  <si>
+    <t>Nejednotný styl, chybějící komentáře a nepřehlednost mohou ztížit údržbu.</t>
+  </si>
+  <si>
+    <t>Všichni</t>
+  </si>
+  <si>
+    <t>Křížková</t>
+  </si>
+  <si>
+    <t>Okon</t>
+  </si>
+  <si>
+    <t>Tkachenko</t>
+  </si>
+  <si>
+    <t>Postupné samostudium, rozdělení oblastí zodpovědnosti (frontend, backend, analýza), využití online tutoriálů a dokumentace.</t>
+  </si>
+  <si>
+    <t>Vyhledání základních kurzů, tvorba jednoduchých testovacích aplikací, průběžné ověřování funkcí.</t>
+  </si>
+  <si>
+    <t>Definovat společný JSON formát a vytvořit základní dokumentaci API (např. Swagger).</t>
+  </si>
+  <si>
+    <t>Zavést jednoduchý workflow (branch → pull request → review), pravidelné zálohy.</t>
+  </si>
+  <si>
+    <t>Konzultace v týmu po každém kroku, průběžná kontrola naplnění požadavků a ověřování logiky aplikace podle zadání.</t>
+  </si>
+  <si>
+    <t>Společná instalace podle sdíleného návodu, dokumentace nastavení.</t>
+  </si>
+  <si>
+    <t>Zavést ruční testování hlavních funkcí, později doplnit jednotkové testy.</t>
+  </si>
+  <si>
+    <t>Použít ORM (Spring Data JPA) a generovat entity podle DB schématu, testovat dotazy.</t>
+  </si>
+  <si>
+    <t>Rozdělit práci na malé úkoly, každý týden vyhodnotit pokrok.</t>
+  </si>
+  <si>
+    <t>Zavést základní pravidla psaní kódu, používat formátování a komentáře.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2226,8 +2329,14 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2240,8 +2349,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF84E290"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFADADAD"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF95DCF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE59EDC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -2292,11 +2425,63 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2323,9 +2508,39 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normální" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2659,24 +2874,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91461C9F-39B2-4D93-9DDB-2C896CD99BC7}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="4" style="1" customWidth="1"/>
     <col min="2" max="2" width="27" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1796875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.6328125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="20.36328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="12.26953125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="1"/>
+    <col min="3" max="3" width="20.19921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="6.796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.9296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="12.265625" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.19921875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="29.5" thickBot="1">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="28.9" thickBot="1">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2702,7 +2917,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="44" thickTop="1">
+    <row r="2" spans="1:8" ht="43.15" thickTop="1">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2728,7 +2943,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="58">
+    <row r="3" spans="1:8" ht="42.75">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -2754,7 +2969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="43.5">
+    <row r="4" spans="1:8" ht="42.75">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -2780,7 +2995,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.5">
+    <row r="5" spans="1:8" ht="42.75">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -2806,7 +3021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="43.5">
+    <row r="6" spans="1:8" ht="42.75">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -2832,7 +3047,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="43.5">
+    <row r="7" spans="1:8" ht="42.75">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -2858,7 +3073,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="43.5">
+    <row r="8" spans="1:8" ht="42.75">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -2884,7 +3099,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="43.5">
+    <row r="9" spans="1:8" ht="42.75">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -2910,7 +3125,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="43.5">
+    <row r="10" spans="1:8" ht="42.75">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -2936,7 +3151,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="43.5">
+    <row r="11" spans="1:8" ht="42.75">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -2962,7 +3177,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="43.5">
+    <row r="12" spans="1:8" ht="42.75">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -2988,7 +3203,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="43.5">
+    <row r="13" spans="1:8" ht="42.75">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -3014,7 +3229,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="58">
+    <row r="14" spans="1:8" ht="57">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -3040,7 +3255,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="58">
+    <row r="15" spans="1:8" ht="57">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -3066,7 +3281,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="43.5">
+    <row r="16" spans="1:8" ht="42.75">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -3092,7 +3307,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="43.5">
+    <row r="17" spans="1:8" ht="42.75">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -3118,7 +3333,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="43.5">
+    <row r="18" spans="1:8" ht="42.75">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -3144,7 +3359,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="43.5">
+    <row r="19" spans="1:8" ht="42.75">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -3170,7 +3385,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="43.5">
+    <row r="20" spans="1:8" ht="42.75">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -3196,7 +3411,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="43.5">
+    <row r="21" spans="1:8" ht="42.75">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -3222,7 +3437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="43.5">
+    <row r="22" spans="1:8" ht="42.75">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -3248,7 +3463,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="43.5">
+    <row r="23" spans="1:8" ht="42.75">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -3274,7 +3489,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="43.5">
+    <row r="24" spans="1:8" ht="42.75">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -3300,7 +3515,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="43.5">
+    <row r="25" spans="1:8" ht="42.75">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -3326,7 +3541,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="43.5">
+    <row r="26" spans="1:8" ht="42.75">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -3352,7 +3567,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="58">
+    <row r="27" spans="1:8" ht="42.75">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -3378,7 +3593,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="29">
+    <row r="28" spans="1:8" ht="28.5">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -3404,7 +3619,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="43.5">
+    <row r="29" spans="1:8" ht="42.75">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -3430,7 +3645,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="43.5">
+    <row r="30" spans="1:8" ht="28.5">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -3456,7 +3671,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="43.5">
+    <row r="31" spans="1:8" ht="42.75">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -3482,7 +3697,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="43.5">
+    <row r="32" spans="1:8" ht="42.75">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -3508,7 +3723,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="43.5">
+    <row r="33" spans="1:8" ht="42.75">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -3555,16 +3770,338 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{669C2F37-BBC9-42D9-B112-B33CEC2CD2BF}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K7" sqref="K7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="2.46484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.265625" customWidth="1"/>
+    <col min="3" max="3" width="44.3984375" customWidth="1"/>
+    <col min="4" max="4" width="17.59765625" customWidth="1"/>
+    <col min="5" max="5" width="18.19921875" customWidth="1"/>
+    <col min="6" max="6" width="18.796875" customWidth="1"/>
+    <col min="7" max="7" width="32.33203125" customWidth="1"/>
+    <col min="8" max="8" width="16.73046875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="45" customHeight="1" thickBot="1">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="36.75" thickTop="1" thickBot="1">
+      <c r="A2" s="10">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="C2" s="11" t="s">
+        <v>225</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="E2" s="10">
+        <v>5</v>
+      </c>
+      <c r="F2" s="10">
+        <v>5</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="36.4" thickBot="1">
+      <c r="A3" s="12">
+        <v>2</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E3" s="12">
+        <v>4</v>
+      </c>
+      <c r="F3" s="12">
+        <v>4</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>249</v>
+      </c>
+      <c r="H3" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="24.4" thickBot="1">
+      <c r="A4" s="14">
+        <v>3</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E4" s="14">
+        <v>3</v>
+      </c>
+      <c r="F4" s="14">
+        <v>4</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="24.4" thickBot="1">
+      <c r="A5" s="16">
+        <v>4</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E5" s="16">
+        <v>3</v>
+      </c>
+      <c r="F5" s="16">
+        <v>4</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="H5" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="36.4" thickBot="1">
+      <c r="A6" s="18">
+        <v>5</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="18">
+        <v>4</v>
+      </c>
+      <c r="F6" s="18">
+        <v>3</v>
+      </c>
+      <c r="G6" s="18" t="s">
+        <v>252</v>
+      </c>
+      <c r="H6" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="24.4" thickBot="1">
+      <c r="A7" s="12">
+        <v>6</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E7" s="10">
+        <v>3</v>
+      </c>
+      <c r="F7" s="10">
+        <v>4</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="H7" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="24.4" thickBot="1">
+      <c r="A8" s="16">
+        <v>7</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>246</v>
+      </c>
+      <c r="E8" s="16">
+        <v>4</v>
+      </c>
+      <c r="F8" s="16">
+        <v>3</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="24.4" thickBot="1">
+      <c r="A9" s="18">
+        <v>8</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="D9" s="18" t="s">
+        <v>247</v>
+      </c>
+      <c r="E9" s="18">
+        <v>4</v>
+      </c>
+      <c r="F9" s="18">
+        <v>3</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>255</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="24.4" thickBot="1">
+      <c r="A10" s="14">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>245</v>
+      </c>
+      <c r="E10" s="14">
+        <v>4</v>
+      </c>
+      <c r="F10" s="14">
+        <v>4</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="24.4" thickBot="1">
+      <c r="A11" s="12">
+        <v>10</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>242</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="10">
+        <v>3</v>
+      </c>
+      <c r="F11" s="10">
+        <v>3</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E1:F1">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD8FEA1A-63FC-4DA3-A792-4375BAD7D9BD}">
   <dimension ref="A1:A177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+    <sheetView topLeftCell="A96" workbookViewId="0">
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="31">
+    <row r="1" spans="1:1" ht="31.9">
       <c r="A1" s="6" t="s">
         <v>107</v>
       </c>
@@ -3777,7 +4314,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="31">
+    <row r="51" spans="1:1" ht="31.9">
       <c r="A51" s="6" t="s">
         <v>140</v>
       </c>
@@ -3834,7 +4371,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:1" ht="31">
+    <row r="65" spans="1:1" ht="31.9">
       <c r="A65" s="6" t="s">
         <v>149</v>
       </c>
@@ -4008,7 +4545,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="106" spans="1:1" ht="31">
+    <row r="106" spans="1:1" ht="31.9">
       <c r="A106" s="6" t="s">
         <v>176</v>
       </c>
@@ -4174,7 +4711,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="145" spans="1:1" ht="31">
+    <row r="145" spans="1:1" ht="31.9">
       <c r="A145" s="6" t="s">
         <v>202</v>
       </c>
@@ -4270,7 +4807,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="168" spans="1:1" ht="31">
+    <row r="168" spans="1:1" ht="31.9">
       <c r="A168" s="6" t="s">
         <v>217</v>
       </c>
@@ -4320,15 +4857,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001D4CC78C6B0F3F4ABC4F6115FC07CE6F" ma:contentTypeVersion="10" ma:contentTypeDescription="Vytvoří nový dokument" ma:contentTypeScope="" ma:versionID="1c4e04370705bc0c5d2dad133a39fa73">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0c73cd0d-0c25-40ab-80ea-3e9f8fc44d59" xmlns:ns3="0cab27e2-5f89-44a4-bd92-116f947691cb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55a60df0a34fa81b36bc9e31f1789d96" ns2:_="" ns3:_="">
     <xsd:import namespace="0c73cd0d-0c25-40ab-80ea-3e9f8fc44d59"/>
@@ -4517,6 +5045,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -4529,14 +5066,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A8A533C-3762-4BB1-B582-2C6C6B2B02E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BFF278DB-B14A-4566-8CED-C39AE8722E74}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4555,6 +5084,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A8A533C-3762-4BB1-B582-2C6C6B2B02E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A19917E-2530-434B-BEC9-4DA316C9818C}">
   <ds:schemaRefs>

</xml_diff>